<commit_message>
updated PvsI with model fitting
</commit_message>
<xml_diff>
--- a/data/respirometry/Fragment_Surface_Area_and_Volume.xlsx
+++ b/data/respirometry/Fragment_Surface_Area_and_Volume.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2917054de0bc48a0/Documents/Barshis_Lab/Field_Work/2023-AS-March-April_American-Samoa/data/Ch2/respirometry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpark\OneDrive\Documents\Barshis_Lab\Field_Work\2023-March-April_American-Samoa\data\respirometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{97DFE2DE-0E91-4DA5-BEA4-4D90DBCCDF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4148094-AA3E-43C1-9BA0-1F97C7FD911F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83307734-82F1-4FD9-9D9A-9552FAE7E32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9021C3D7-74DC-4965-ADF5-F50A19582A88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9021C3D7-74DC-4965-ADF5-F50A19582A88}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>std</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Buoyant_Weight(g)</t>
+  </si>
+  <si>
+    <t>effective_volume</t>
   </si>
 </sst>
 </file>
@@ -570,20 +573,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695A72CA-5C65-40AB-91E7-BF50853B35EC}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.08984375" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" customWidth="1"/>
+    <col min="1" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -602,8 +606,11 @@
       <c r="F1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -623,8 +630,12 @@
       <c r="F2">
         <v>14.17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <f>(154.4 - (F2 / 1.025)) / 1000</f>
+        <v>0.14057560975609756</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -644,8 +655,12 @@
       <c r="F3">
         <v>10.65</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <f t="shared" ref="G3:G23" si="1">(154.4 - (F3 / 1.025)) / 1000</f>
+        <v>0.14400975609756098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -665,8 +680,12 @@
       <c r="F4">
         <v>8.34</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.14626341463414635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -686,8 +705,12 @@
       <c r="F5">
         <v>4.47</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.15003902439024389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -707,8 +730,12 @@
       <c r="F6">
         <v>8.23</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.14637073170731707</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -728,8 +755,12 @@
       <c r="F7">
         <v>8.0299999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.14656585365853658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -749,8 +780,12 @@
       <c r="F8">
         <v>9.67</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.14496585365853659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -770,8 +805,12 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.15440000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -791,8 +830,12 @@
       <c r="F10">
         <v>12.09</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.1426048780487805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -812,8 +855,12 @@
       <c r="F11">
         <v>12.36</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.14234146341463416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -833,8 +880,12 @@
       <c r="F12">
         <v>6.84</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.14772682926829267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -854,8 +905,12 @@
       <c r="F13">
         <v>7.55</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.14703414634146342</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -875,8 +930,12 @@
       <c r="F14">
         <v>6.81</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.1477560975609756</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -896,8 +955,12 @@
       <c r="F15">
         <v>9.09</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.14553170731707318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -917,8 +980,12 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0.15440000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -938,8 +1005,12 @@
       <c r="F17">
         <v>9.6300000000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.14500487804878048</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -959,8 +1030,12 @@
       <c r="F18">
         <v>5.28</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.14924878048780488</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -980,8 +1055,12 @@
       <c r="F19">
         <v>7.66</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0.1469268292682927</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1001,8 +1080,12 @@
       <c r="F20">
         <v>12.82</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0.14189268292682927</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1022,8 +1105,12 @@
       <c r="F21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0.14464390243902439</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1043,8 +1130,12 @@
       <c r="F22">
         <v>11.76</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0.1429268292682927</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1063,6 +1154,10 @@
       </c>
       <c r="F23">
         <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0.15440000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1079,16 +1174,16 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1102,7 +1197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1124,7 +1219,7 @@
         <v>4.5528000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1146,7 +1241,7 @@
         <v>3.0114559048185644E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1161,7 +1256,7 @@
         <v>4.5111999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1172,7 +1267,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1279,7 @@
         <v>24.784747847478474</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1291,7 @@
         <v>15.179669653839396</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1303,7 @@
         <v>15.610173958882445</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1220,7 +1315,7 @@
         <v>16.012124406958357</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1232,7 +1327,7 @@
         <v>16.007731505886486</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1339,7 @@
         <v>20.040414689861183</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1256,7 +1351,7 @@
         <v>24.791337199086275</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1268,7 +1363,7 @@
         <v>22.206114918292037</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1375,7 @@
         <v>25.654542259708311</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1292,7 +1387,7 @@
         <v>24.912141978562644</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1304,7 +1399,7 @@
         <v>20.826743981725532</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1411,7 @@
         <v>16.071428571428569</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1328,7 +1423,7 @@
         <v>22.476278334211916</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1340,7 +1435,7 @@
         <v>24.48603057459146</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1352,7 +1447,7 @@
         <v>14.889738183096117</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1364,7 +1459,7 @@
         <v>22.22807942365138</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1376,7 +1471,7 @@
         <v>25.294324371815147</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1388,7 +1483,7 @@
         <v>18.516078017923036</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1400,7 +1495,7 @@
         <v>32.322966086803724</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>43</v>
       </c>
@@ -1409,7 +1504,7 @@
         <v>21.174245577042232</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>